<commit_message>
Reading Reports 1,2 and 3 update
</commit_message>
<xml_diff>
--- a/src/senaite/instruments/tests/files/instruments/agilent/flameatomic/flameatomic_QC_and_blank.xlsx
+++ b/src/senaite/instruments/tests/files/instruments/agilent/flameatomic/flameatomic_QC_and_blank.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t xml:space="preserve">Analyste</t>
   </si>
@@ -58,19 +58,28 @@
     <t xml:space="preserve">mg/L</t>
   </si>
   <si>
+    <t xml:space="preserve">QC-001-001</t>
+  </si>
+  <si>
     <t xml:space="preserve">QC-002-001</t>
   </si>
   <si>
-    <t xml:space="preserve">QC-001-001</t>
-  </si>
-  <si>
     <t xml:space="preserve">Méthode: Au Aqua Regia Echelle2 (Flamme)</t>
   </si>
   <si>
+    <t xml:space="preserve">QC-001-002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QC-002-002</t>
+  </si>
+  <si>
     <t xml:space="preserve">Méthode: Au Aqua Regia Echelle3 (Flamme)</t>
   </si>
   <si>
-    <t xml:space="preserve">QC-002–001</t>
+    <t xml:space="preserve">QC-001-003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QC-002-003</t>
   </si>
 </sst>
 </file>
@@ -85,6 +94,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -106,6 +116,7 @@
       <color rgb="FF434343"/>
       <name val="Open Sans"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -281,10 +292,10 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+      <selection pane="topLeft" activeCell="P27" activeCellId="0" sqref="P27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.18"/>
   </cols>
@@ -521,7 +532,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B15" s="6" t="n">
         <v>9.8</v>
@@ -551,7 +562,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B16" s="6" t="n">
         <v>8.7</v>
@@ -623,7 +634,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -631,7 +642,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B21" s="6" t="n">
         <v>15</v>
@@ -661,7 +672,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B22" s="6" t="n">
         <v>14</v>

</xml_diff>